<commit_message>
25th june ml commit
</commit_message>
<xml_diff>
--- a/ML/Jupyter Notebooks/vineday_3.xlsx
+++ b/ML/Jupyter Notebooks/vineday_3.xlsx
@@ -137,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,12 +166,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,16 +217,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,8 +245,8 @@
   </sheetPr>
   <dimension ref="A1:AF23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG1" activeCellId="0" sqref="AG1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ10" activeCellId="0" sqref="AJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -363,7 +353,7 @@
       <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
@@ -474,7 +464,7 @@
         <v>6000</v>
       </c>
       <c r="AF2" s="0" t="n">
-        <v>58</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,7 +562,7 @@
         <v>6000</v>
       </c>
       <c r="AF3" s="0" t="n">
-        <v>24</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,7 +660,7 @@
         <v>6000</v>
       </c>
       <c r="AF4" s="0" t="n">
-        <v>29</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,7 +758,7 @@
         <v>6000</v>
       </c>
       <c r="AF5" s="0" t="n">
-        <v>33</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +856,7 @@
         <v>6000</v>
       </c>
       <c r="AF6" s="0" t="n">
-        <v>30</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,7 +954,7 @@
         <v>6233</v>
       </c>
       <c r="AF7" s="0" t="n">
-        <v>40</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,7 +1052,7 @@
         <v>6267</v>
       </c>
       <c r="AF8" s="0" t="n">
-        <v>58</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,7 +1150,7 @@
         <v>6267</v>
       </c>
       <c r="AF9" s="0" t="n">
-        <v>64</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,7 +1248,7 @@
         <v>6267</v>
       </c>
       <c r="AF10" s="0" t="n">
-        <v>52</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,7 +1346,7 @@
         <v>6033</v>
       </c>
       <c r="AF11" s="0" t="n">
-        <v>71</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,7 +1444,7 @@
         <v>6067</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>49</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,7 +1542,7 @@
         <v>6100</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>34</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,7 +1640,7 @@
         <v>6133</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>62</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,7 +1738,7 @@
         <v>6167</v>
       </c>
       <c r="AF15" s="0" t="n">
-        <v>27</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1836,7 @@
         <v>6200</v>
       </c>
       <c r="AF16" s="0" t="n">
-        <v>80</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,7 +1934,7 @@
         <v>6233</v>
       </c>
       <c r="AF17" s="0" t="n">
-        <v>40</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +2032,7 @@
         <v>6267</v>
       </c>
       <c r="AF18" s="0" t="n">
-        <v>58</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,7 +2130,7 @@
         <v>6300</v>
       </c>
       <c r="AF19" s="0" t="n">
-        <v>77</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2238,7 +2228,7 @@
         <v>6233</v>
       </c>
       <c r="AF20" s="0" t="n">
-        <v>40</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2336,7 +2326,7 @@
         <v>6267</v>
       </c>
       <c r="AF21" s="0" t="n">
-        <v>54</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,7 +2424,7 @@
         <v>6300</v>
       </c>
       <c r="AF22" s="0" t="n">
-        <v>79</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,7 +2522,7 @@
         <v>6233</v>
       </c>
       <c r="AF23" s="0" t="n">
-        <v>40</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
returned tons to predictions
</commit_message>
<xml_diff>
--- a/ML/Jupyter Notebooks/vineday_3.xlsx
+++ b/ML/Jupyter Notebooks/vineday_3.xlsx
@@ -246,7 +246,7 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ10" activeCellId="0" sqref="AJ10"/>
+      <selection pane="topLeft" activeCell="AL15" activeCellId="0" sqref="AL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,7 +464,7 @@
         <v>6000</v>
       </c>
       <c r="AF2" s="0" t="n">
-        <v>1.16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,7 +562,7 @@
         <v>6000</v>
       </c>
       <c r="AF3" s="0" t="n">
-        <v>0.48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,7 +660,7 @@
         <v>6000</v>
       </c>
       <c r="AF4" s="0" t="n">
-        <v>0.58</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,7 +758,7 @@
         <v>6000</v>
       </c>
       <c r="AF5" s="0" t="n">
-        <v>0.66</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,7 +856,7 @@
         <v>6000</v>
       </c>
       <c r="AF6" s="0" t="n">
-        <v>0.6</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,7 +954,7 @@
         <v>6233</v>
       </c>
       <c r="AF7" s="0" t="n">
-        <v>0.8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,7 +1052,7 @@
         <v>6267</v>
       </c>
       <c r="AF8" s="0" t="n">
-        <v>1.16</v>
+        <v>30.9090909090909</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,7 +1150,7 @@
         <v>6267</v>
       </c>
       <c r="AF9" s="0" t="n">
-        <v>1.28</v>
+        <v>36.3636363636364</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,7 +1248,7 @@
         <v>6267</v>
       </c>
       <c r="AF10" s="0" t="n">
-        <v>1.04</v>
+        <v>25.4545454545455</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,7 +1346,7 @@
         <v>6033</v>
       </c>
       <c r="AF11" s="0" t="n">
-        <v>1.42</v>
+        <v>42.7272727272727</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1444,7 +1444,7 @@
         <v>6067</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>0.98</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,7 +1542,7 @@
         <v>6100</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>0.68</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,7 +1640,7 @@
         <v>6133</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>1.24</v>
+        <v>34.5454545454545</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,7 +1738,7 @@
         <v>6167</v>
       </c>
       <c r="AF15" s="0" t="n">
-        <v>0.54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1836,7 @@
         <v>6200</v>
       </c>
       <c r="AF16" s="0" t="n">
-        <v>1.6</v>
+        <v>32.7272727272727</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,7 +1934,7 @@
         <v>6233</v>
       </c>
       <c r="AF17" s="0" t="n">
-        <v>0.8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2032,7 @@
         <v>6267</v>
       </c>
       <c r="AF18" s="0" t="n">
-        <v>1.16</v>
+        <v>30.9090909090909</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2130,7 @@
         <v>6300</v>
       </c>
       <c r="AF19" s="0" t="n">
-        <v>1.54</v>
+        <v>48.1818181818182</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2228,7 +2228,7 @@
         <v>6233</v>
       </c>
       <c r="AF20" s="0" t="n">
-        <v>0.8</v>
+        <v>14.5454545454545</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2326,7 +2326,7 @@
         <v>6267</v>
       </c>
       <c r="AF21" s="0" t="n">
-        <v>1.08</v>
+        <v>27.2727272727273</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2424,7 +2424,7 @@
         <v>6300</v>
       </c>
       <c r="AF22" s="0" t="n">
-        <v>1.58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,7 +2522,7 @@
         <v>6233</v>
       </c>
       <c r="AF23" s="0" t="n">
-        <v>0.8</v>
+        <v>14.5454545454545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>